<commit_message>
Plan de test - application complété pour l'accordeur
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Plan de test application.xlsx
+++ b/Documentation/Tests/Plan de test application.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Gabarit" sheetId="1" r:id="rId1"/>
-    <sheet name="Autocorrélation " sheetId="3" r:id="rId2"/>
+    <sheet name="Accordeur" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -84,25 +84,57 @@
     <t>Accordeur</t>
   </si>
   <si>
-    <t>Pour un réglage de 5 kHz, injecter une sinus de 2,5 kHz</t>
-  </si>
-  <si>
-    <t>Pour un réglage de 5 kHz, injecter une sinus de 5 kHz</t>
-  </si>
-  <si>
-    <t>Pour un réglage de 5 kHz, injecter une sinus de 10 kHz</t>
-  </si>
-  <si>
-    <t>DEL de droite allumée</t>
-  </si>
-  <si>
-    <t>DEL de gauche allumée</t>
-  </si>
-  <si>
-    <t>DEL du centre allumée</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>DEL de gauche (DEL 2) allumée</t>
+  </si>
+  <si>
+    <t>DEL du centre (DEL 1) allumée</t>
+  </si>
+  <si>
+    <t>DEL de droite (DEL 0) allumée</t>
+  </si>
+  <si>
+    <t>Réussite</t>
+  </si>
+  <si>
+    <t>DEL du centre (DEL 0) allumée</t>
+  </si>
+  <si>
+    <t>*Après fenêtrage 
+d'autocorrélation</t>
+  </si>
+  <si>
+    <t>La fonction peut être implémentée
+ de deux façon différentes, dépendamment 
+de l'application. En effet, un fenêtrage 
+après l'autocorrélation s'avère préférable 
+pour analyser les hautes fréquences par rapport 
+à la fréquence de référence. D'une autre part, 
+le fenêtrage est non favorable en ce qui concerne
+ le respect précis des bornes et un peu sur 
+l'aspect des petites fréquences. Pour notre 
+application, l'absence de fenêtrage s'avère une 
+meilleure utilité pour un accordeur de guitare.</t>
+  </si>
+  <si>
+    <t>Pour un réglage de 4 kHz, injecter une sinus de 2 kHz</t>
+  </si>
+  <si>
+    <t>Pour un réglage de 4 kHz, injecter une sinus de 4 kHz</t>
+  </si>
+  <si>
+    <t>*Avec et sans fenêtrage</t>
+  </si>
+  <si>
+    <t>*Avec et sans fenêtrage 
+entre 4kHz et 8kHz très 
+instable, non préférable 
+pour haute fréquence</t>
+  </si>
+  <si>
+    <t>Pour un réglage de 4 kHz, injecter une sinus de 8 kHz</t>
   </si>
 </sst>
 </file>
@@ -667,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -706,68 +738,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,14 +776,83 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,24 +866,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1170,16 +1208,16 @@
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
-      <c r="F2" s="41" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1188,16 +1226,16 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="F3" s="45" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="F3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
@@ -1206,22 +1244,22 @@
       <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="49" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="18" t="s">
+      <c r="F5" s="39"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="43"/>
       <c r="L5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1236,181 +1274,181 @@
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="33"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
-      <c r="O6" s="36"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>2</v>
       </c>
       <c r="B7" s="34"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="41"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="36"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="O7" s="37"/>
+      <c r="O7" s="20"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>3</v>
       </c>
       <c r="B8" s="34"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="34"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="36"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-      <c r="O8" s="37"/>
+      <c r="O8" s="20"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>4</v>
       </c>
       <c r="B9" s="34"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="26"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="41"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="36"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-      <c r="O9" s="37"/>
+      <c r="O9" s="20"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>5</v>
       </c>
       <c r="B10" s="34"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="41"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="36"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="O10" s="37"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>6</v>
       </c>
       <c r="B11" s="34"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="41"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="O11" s="37"/>
+      <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>7</v>
       </c>
       <c r="B12" s="34"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="34"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="36"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="O12" s="37"/>
+      <c r="O12" s="20"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>8</v>
       </c>
       <c r="B13" s="34"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="O13" s="37"/>
+      <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>9</v>
       </c>
       <c r="B14" s="34"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="41"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-      <c r="O14" s="37"/>
+      <c r="O14" s="20"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>10</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
-      <c r="O15" s="38"/>
+      <c r="O15" s="21"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -1425,6 +1463,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="O6:O15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -1441,30 +1503,6 @@
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1475,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,7 +1524,7 @@
     <col min="12" max="12" width="19.28515625" customWidth="1"/>
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1494,16 +1532,16 @@
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
-      <c r="F2" s="41" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1512,38 +1550,38 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="F3" s="45" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="F3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
       <c r="L5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1555,24 +1593,24 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>1</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="60"/>
-      <c r="O6" s="57"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
+      <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1583,18 +1621,24 @@
       </c>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="O7" s="37"/>
+      <c r="M7" s="17"/>
+      <c r="O7" s="60" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1605,18 +1649,22 @@
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
-      <c r="E8" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="O8" s="37"/>
+      <c r="E8" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="17"/>
+      <c r="O8" s="61"/>
     </row>
     <row r="9" spans="1:15" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1627,112 +1675,149 @@
       </c>
       <c r="C9" s="55"/>
       <c r="D9" s="55"/>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="O9" s="37"/>
-    </row>
-    <row r="10" spans="1:15" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="61"/>
+    </row>
+    <row r="10" spans="1:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1.4</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="O10" s="37"/>
+      <c r="M10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="61"/>
     </row>
     <row r="11" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>1.5</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C11" s="55"/>
       <c r="D11" s="55"/>
-      <c r="E11" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="O11" s="37"/>
-    </row>
-    <row r="12" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="61"/>
+    </row>
+    <row r="12" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1.6</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="O12" s="37"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="61"/>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:K5"/>
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="O7:O12"/>
     <mergeCell ref="B12:D12"/>
@@ -1749,19 +1834,6 @@
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>